<commit_message>
Author                         : Aashish Sharma Files Modified                 : AashishSharma.xlsx Description                    : Updated Task Breakdown
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aashish sharma\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Desktop\SVN\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Story ID</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Creating DAO's for all Queries</t>
+  </si>
+  <si>
+    <t>T-12</t>
   </si>
 </sst>
 </file>
@@ -289,6 +292,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,10 +311,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G61"/>
+  <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H62" sqref="A41:H62"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,12 +631,12 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8">
-        <f>SUM(E3:E19)</f>
-        <v>51</v>
+      <c r="B3" s="10">
+        <f>SUM(E3:E18)</f>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -651,8 +654,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="9"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
@@ -664,13 +667,13 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G61" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G60" si="0">E4-F4</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
@@ -687,8 +690,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -702,10 +705,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>16</v>
@@ -718,8 +721,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>24</v>
@@ -734,8 +737,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>26</v>
@@ -750,8 +753,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
         <v>27</v>
@@ -766,10 +769,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>36</v>
@@ -784,10 +787,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>38</v>
@@ -802,10 +805,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>37</v>
@@ -820,10 +823,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>39</v>
@@ -838,88 +841,78 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="2">
-        <v>1</v>
+      <c r="A18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="7">
+        <v>6</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <f>E17-F18</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="12">
-        <v>6</v>
-      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f>E18-F19</f>
-        <v>1</v>
-      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
@@ -930,26 +923,36 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="10">
+        <f>SUM(E21:E35)</f>
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="8">
-        <f>SUM(E22:E36)</f>
-        <v>42</v>
-      </c>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -961,13 +964,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -979,95 +982,95 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="E26" s="6">
+        <v>2</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="11">
-        <v>2</v>
+        <v>28</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E28" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E29" s="2">
         <v>6</v>
@@ -1079,13 +1082,13 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -1097,67 +1100,67 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="E31" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E32" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E34" s="2">
         <v>1</v>
@@ -1169,37 +1172,31 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="E35" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="2">
-        <v>6</v>
-      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,24 +1487,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A3:A19"/>
-    <mergeCell ref="A22:A35"/>
-    <mergeCell ref="B3:B19"/>
-    <mergeCell ref="B22:B35"/>
+    <mergeCell ref="A3:A18"/>
+    <mergeCell ref="A21:A34"/>
+    <mergeCell ref="B3:B18"/>
+    <mergeCell ref="B21:B34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Author               :  Aashish Sharma Files Modified       :  AashishSharma.xlsx Description          :  Updated after reviewed by Ruchi Ma'am
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Story ID</t>
   </si>
@@ -53,12 +53,6 @@
     <t>SSDMS-51</t>
   </si>
   <si>
-    <t>Understanding the 'WHY' of the story.</t>
-  </si>
-  <si>
-    <t>Understanding forward and backward linkages.</t>
-  </si>
-  <si>
     <t>T-01</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>T-07</t>
   </si>
   <si>
-    <t>Encorporate Code Review changes</t>
-  </si>
-  <si>
     <t>T-08</t>
   </si>
   <si>
@@ -110,18 +101,6 @@
     <t>ii) BootStrap - how to design using bootstrap</t>
   </si>
   <si>
-    <t xml:space="preserve">iii) Writing the dynamic SQL queries </t>
-  </si>
-  <si>
-    <t>Making the Controllers,Services for the SQL queries</t>
-  </si>
-  <si>
-    <t>ii) Collaborating with the frontend team(deciding the controller's name and type of data to be outputted to every query)</t>
-  </si>
-  <si>
-    <t>Debugging</t>
-  </si>
-  <si>
     <t>T-09</t>
   </si>
   <si>
@@ -131,31 +110,55 @@
     <t>T-11</t>
   </si>
   <si>
-    <t>Finalzing the required fields of TP,AB and grouping of fields in Accordions</t>
-  </si>
-  <si>
-    <t>Designing of page structure using HTML</t>
-  </si>
-  <si>
-    <t>Integrating and creating fields using AngularJS</t>
-  </si>
-  <si>
-    <t>Adding Design using Bootstrap</t>
-  </si>
-  <si>
-    <t>Adding CSS to the page</t>
-  </si>
-  <si>
     <t>Buffer Time</t>
   </si>
   <si>
-    <t>Creating DTO's for all Queries</t>
-  </si>
-  <si>
-    <t>Creating DAO's for all Queries</t>
-  </si>
-  <si>
     <t>T-12</t>
+  </si>
+  <si>
+    <t>Develop technical understanding</t>
+  </si>
+  <si>
+    <t>Design page structure using HTML</t>
+  </si>
+  <si>
+    <t>Incorporate Code Review changes</t>
+  </si>
+  <si>
+    <t>Understand the 'WHY' of the story.</t>
+  </si>
+  <si>
+    <t>Understand forward and backward linkages.</t>
+  </si>
+  <si>
+    <t>Finalze the required fields of TP,AB and grouping of fields in Accordions</t>
+  </si>
+  <si>
+    <t>Add Design using Bootstrap</t>
+  </si>
+  <si>
+    <t>Integrate and creating fields using AngularJS</t>
+  </si>
+  <si>
+    <t>Add CSS to the page</t>
+  </si>
+  <si>
+    <t>ii) Collaborate with the frontend team(deciding the controller's name and type of data to be outputted to every query)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iii) Write dynamic SQL queries </t>
+  </si>
+  <si>
+    <t>Design the Controllers,Services for the SQL queries</t>
+  </si>
+  <si>
+    <t>Create DTO's for all Queries</t>
+  </si>
+  <si>
+    <t>Create DAO's for all Queries</t>
+  </si>
+  <si>
+    <t>Debugg</t>
   </si>
 </sst>
 </file>
@@ -593,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,13 +639,13 @@
       </c>
       <c r="B3" s="10">
         <f>SUM(E3:E18)</f>
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -657,10 +660,10 @@
       <c r="A4" s="9"/>
       <c r="B4" s="11"/>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -675,10 +678,10 @@
       <c r="A5" s="9"/>
       <c r="B5" s="11"/>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
@@ -689,11 +692,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="11"/>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>35</v>
@@ -708,10 +711,10 @@
       <c r="A7" s="9"/>
       <c r="B7" s="11"/>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -725,7 +728,7 @@
       <c r="B8" s="11"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
         <v>6</v>
@@ -741,7 +744,7 @@
       <c r="B9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
         <v>4</v>
@@ -757,7 +760,7 @@
       <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E10" s="2">
         <v>6</v>
@@ -772,10 +775,10 @@
       <c r="A11" s="9"/>
       <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -790,10 +793,10 @@
       <c r="A12" s="9"/>
       <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="2">
         <v>6</v>
@@ -808,7 +811,7 @@
       <c r="A13" s="9"/>
       <c r="B13" s="11"/>
       <c r="C13" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>37</v>
@@ -826,10 +829,10 @@
       <c r="A14" s="9"/>
       <c r="B14" s="11"/>
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -844,10 +847,10 @@
       <c r="A15" s="9"/>
       <c r="B15" s="11"/>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -862,10 +865,10 @@
       <c r="A16" s="9"/>
       <c r="B16" s="11"/>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -880,10 +883,10 @@
       <c r="A17" s="9"/>
       <c r="B17" s="11"/>
       <c r="C17" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
@@ -895,10 +898,10 @@
       <c r="A18" s="9"/>
       <c r="B18" s="12"/>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
@@ -928,13 +931,13 @@
       </c>
       <c r="B21" s="10">
         <f>SUM(E21:E35)</f>
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
@@ -949,10 +952,10 @@
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -967,10 +970,10 @@
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -985,10 +988,10 @@
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1002,7 +1005,7 @@
       <c r="B25" s="11"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -1018,7 +1021,7 @@
       <c r="B26" s="11"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E26" s="6">
         <v>2</v>
@@ -1034,7 +1037,7 @@
       <c r="B27" s="11"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2">
         <v>4</v>
@@ -1049,10 +1052,10 @@
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E28" s="2">
         <v>6</v>
@@ -1067,10 +1070,10 @@
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E29" s="2">
         <v>6</v>
@@ -1085,10 +1088,10 @@
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -1103,10 +1106,10 @@
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E31" s="2">
         <v>4</v>
@@ -1121,10 +1124,10 @@
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
         <v>2</v>
@@ -1139,10 +1142,10 @@
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>
@@ -1157,10 +1160,10 @@
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E34" s="2">
         <v>1</v>
@@ -1176,15 +1179,15 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E35" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author             :  Aashish Sharma Description        :  Updated Today's Task in TasksBreakDown/AashishSharma.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,10 +650,12 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
       <c r="G3" s="2">
         <f>E3-F3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -668,10 +670,12 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2">
         <f t="shared" ref="G4:G60" si="0">E4-F4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -686,10 +690,12 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -942,10 +948,12 @@
       <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2">
+        <v>1</v>
+      </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -960,10 +968,12 @@
       <c r="E22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,10 +988,12 @@
       <c r="E23" s="2">
         <v>1</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,10 +1022,12 @@
       <c r="E25" s="2">
         <v>1</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1026,10 +1040,12 @@
       <c r="E26" s="6">
         <v>2</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="2">
+        <v>2</v>
+      </c>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1060,10 +1076,12 @@
       <c r="E28" s="2">
         <v>6</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,10 +1096,12 @@
       <c r="E29" s="2">
         <v>6</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1096,10 +1116,12 @@
       <c r="E30" s="2">
         <v>6</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author        : Aashish Sharma Files Modified: AashishSharma.xlsx Description   : Updated TaskBreakDown sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,10 +1058,12 @@
       <c r="E27" s="2">
         <v>4</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2">
+        <v>3</v>
+      </c>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1077,11 +1079,11 @@
         <v>6</v>
       </c>
       <c r="F28" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,11 +1099,11 @@
         <v>6</v>
       </c>
       <c r="F29" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1117,11 +1119,11 @@
         <v>6</v>
       </c>
       <c r="F30" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author       :  Aashish Sharma Desciption   :  Updated TaskBreakdown Sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Desktop\SVN\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Story ID</t>
   </si>
@@ -159,6 +159,21 @@
   </si>
   <si>
     <t>Debugg</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In-Dev</t>
+  </si>
+  <si>
+    <t>Not-Started</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +207,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -280,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -294,9 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -314,12 +356,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G60"/>
+  <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="H18" sqref="H6:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,9 +694,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -632,12 +719,15 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="H2" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f>SUM(E3:E18)</f>
         <v>43</v>
       </c>
@@ -657,10 +747,13 @@
         <f>E3-F3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="11"/>
+      <c r="H3" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -674,13 +767,16 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G60" si="0">E4-F4</f>
+        <f t="shared" ref="G4:G35" si="0">E4-F4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="11"/>
+      <c r="H4" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -697,10 +793,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="11"/>
+      <c r="H5" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -712,10 +811,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="11"/>
+      <c r="H6" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
@@ -724,14 +826,12 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="11"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -744,10 +844,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="11"/>
+      <c r="H8" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>23</v>
@@ -760,10 +863,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="11"/>
+      <c r="H9" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -776,10 +882,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="11"/>
+      <c r="H10" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
@@ -794,10 +903,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="11"/>
+      <c r="H11" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -812,10 +924,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="11"/>
+      <c r="H12" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
@@ -830,10 +945,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="11"/>
+      <c r="H13" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
@@ -848,10 +966,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="11"/>
+      <c r="H14" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -866,10 +987,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="11"/>
+      <c r="H15" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
@@ -884,10 +1008,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="11"/>
+      <c r="H16" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
@@ -899,14 +1026,17 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="12"/>
+      <c r="H17" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="11"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>2</v>
       </c>
       <c r="F18" s="2"/>
@@ -914,8 +1044,11 @@
         <f>E17-F18</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -923,7 +1056,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -931,11 +1064,11 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="9">
         <f>SUM(E21:E35)</f>
         <v>38</v>
       </c>
@@ -955,10 +1088,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="H21" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
@@ -975,10 +1111,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="H22" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
@@ -995,10 +1134,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
+      <c r="H23" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1011,10 +1153,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
+      <c r="H24" s="18"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -1029,15 +1172,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
+      <c r="H25" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="17">
         <v>2</v>
       </c>
       <c r="F26" s="2">
@@ -1047,10 +1193,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
+      <c r="H26" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>40</v>
@@ -1065,10 +1214,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
+      <c r="H27" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
@@ -1085,10 +1237,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
+      <c r="H28" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
@@ -1105,10 +1260,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
+      <c r="H29" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
@@ -1125,10 +1283,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
+      <c r="H30" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1143,10 +1304,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
+      <c r="H31" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1161,10 +1325,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+      <c r="H32" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1179,10 +1346,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="H33" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
@@ -1197,8 +1367,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1213,162 +1386,140 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="13">
+        <f>SUM(B21,B3)</f>
+        <v>81</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F37" s="14">
+        <f>SUM(F3:F35)</f>
+        <v>25</v>
+      </c>
+      <c r="G37" s="15">
+        <f>SUM(G3:G35)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
@@ -1377,10 +1528,7 @@
       <c r="D49" s="3"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
@@ -1389,10 +1537,7 @@
       <c r="D50" s="3"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
@@ -1401,10 +1546,7 @@
       <c r="D51" s="3"/>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
-      <c r="G51" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
@@ -1413,10 +1555,7 @@
       <c r="D52" s="3"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
-      <c r="G52" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G52" s="2"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
@@ -1425,10 +1564,7 @@
       <c r="D53" s="3"/>
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
-      <c r="G53" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
@@ -1437,10 +1573,7 @@
       <c r="D54" s="3"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
-      <c r="G54" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G54" s="2"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
@@ -1449,10 +1582,7 @@
       <c r="D55" s="3"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-      <c r="G55" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
@@ -1461,10 +1591,7 @@
       <c r="D56" s="3"/>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
-      <c r="G56" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
@@ -1473,10 +1600,7 @@
       <c r="D57" s="3"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
-      <c r="G57" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
@@ -1485,10 +1609,7 @@
       <c r="D58" s="3"/>
       <c r="E58" s="2"/>
       <c r="F58" s="2"/>
-      <c r="G58" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
@@ -1497,10 +1618,7 @@
       <c r="D59" s="3"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-      <c r="G59" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
@@ -1509,10 +1627,7 @@
       <c r="D60" s="3"/>
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
-      <c r="G60" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G60" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Author              : Aashish Sharma Description         : Updated TaskBreakdown sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -341,6 +341,17 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,17 +367,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="H18" sqref="H6:H18"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,15 +719,15 @@
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="11" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="18">
         <f>SUM(E3:E18)</f>
         <v>43</v>
       </c>
@@ -747,13 +747,13 @@
         <f>E3-F3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -770,13 +770,13 @@
         <f t="shared" ref="G4:G35" si="0">E4-F4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -793,13 +793,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -811,13 +811,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
@@ -827,11 +827,11 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -844,13 +844,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>23</v>
@@ -863,13 +863,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -882,13 +882,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
@@ -903,13 +903,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -924,13 +924,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
@@ -945,13 +945,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
@@ -966,13 +966,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -987,13 +987,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1008,13 +1008,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1026,13 +1026,13 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="20"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1044,7 +1044,7 @@
         <f>E17-F18</f>
         <v>1</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H18" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1065,10 +1065,10 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="18">
         <f>SUM(E21:E35)</f>
         <v>38</v>
       </c>
@@ -1088,13 +1088,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1111,13 +1111,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1134,13 +1134,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1153,11 +1153,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="18"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -1172,18 +1172,18 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="12">
         <v>2</v>
       </c>
       <c r="F26" s="2">
@@ -1193,13 +1193,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>40</v>
@@ -1208,19 +1208,19 @@
         <v>4</v>
       </c>
       <c r="F27" s="2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H27" s="19" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
@@ -1231,19 +1231,19 @@
         <v>6</v>
       </c>
       <c r="F28" s="2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H28" s="19" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
@@ -1254,19 +1254,19 @@
         <v>6</v>
       </c>
       <c r="F29" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H29" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
@@ -1277,19 +1277,19 @@
         <v>6</v>
       </c>
       <c r="F30" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H30" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1299,18 +1299,20 @@
       <c r="E31" s="2">
         <v>4</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2">
+        <v>4</v>
+      </c>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1320,18 +1322,20 @@
       <c r="E32" s="2">
         <v>2</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H32" s="20" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1346,13 +1350,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="H33" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
@@ -1367,7 +1371,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H34" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1386,7 +1390,7 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="15" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1398,28 +1402,28 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="20" t="s">
+      <c r="H36" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="8">
         <f>SUM(B21,B3)</f>
         <v>81</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="14">
+      <c r="F37" s="9">
         <f>SUM(F3:F35)</f>
-        <v>25</v>
-      </c>
-      <c r="G37" s="15">
+        <v>34</v>
+      </c>
+      <c r="G37" s="10">
         <f>SUM(G3:G35)</f>
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Author Id                   : Aashish Sharma Description                 : Updated Task Breakdown sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/AashishSharma.xlsx
+++ b/TeamDetails/TasksBreakDown/AashishSharma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t>Story ID</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>In-Dev</t>
   </si>
   <si>
     <t>Not-Started</t>
@@ -325,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,7 +347,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -682,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,10 +720,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="17">
         <f>SUM(E3:E18)</f>
         <v>43</v>
       </c>
@@ -752,8 +748,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -775,8 +771,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -798,8 +794,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -811,13 +807,13 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="15" t="s">
-        <v>49</v>
+      <c r="H6" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
@@ -827,11 +823,11 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="15"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3" t="s">
         <v>21</v>
@@ -844,13 +840,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>49</v>
+      <c r="H8" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3" t="s">
         <v>23</v>
@@ -863,13 +859,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H9" s="15" t="s">
-        <v>49</v>
+      <c r="H9" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -882,13 +878,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>49</v>
+      <c r="H10" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
@@ -903,13 +899,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>49</v>
+      <c r="H11" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
@@ -924,13 +920,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>49</v>
+      <c r="H12" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="19"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="2" t="s">
         <v>20</v>
       </c>
@@ -945,13 +941,13 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>49</v>
+      <c r="H13" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="19"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
@@ -966,13 +962,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>49</v>
+      <c r="H14" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="19"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
@@ -987,13 +983,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>49</v>
+      <c r="H15" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="19"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1008,13 +1004,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H16" s="15" t="s">
-        <v>49</v>
+      <c r="H16" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="19"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1026,13 +1022,13 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="15" t="s">
-        <v>49</v>
+      <c r="H17" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="19"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1044,8 +1040,8 @@
         <f>E17-F18</f>
         <v>1</v>
       </c>
-      <c r="H18" s="15" t="s">
-        <v>49</v>
+      <c r="H18" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1065,10 +1061,10 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="17">
         <f>SUM(E21:E35)</f>
         <v>38</v>
       </c>
@@ -1093,8 +1089,8 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1116,8 +1112,8 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="2" t="s">
         <v>11</v>
       </c>
@@ -1139,8 +1135,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1156,8 +1152,8 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
         <v>22</v>
@@ -1177,8 +1173,8 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3" t="s">
         <v>39</v>
@@ -1198,8 +1194,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="19"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3" t="s">
         <v>40</v>
@@ -1208,19 +1204,19 @@
         <v>4</v>
       </c>
       <c r="F27" s="2">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="19"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="2" t="s">
         <v>15</v>
       </c>
@@ -1231,19 +1227,19 @@
         <v>6</v>
       </c>
       <c r="F28" s="2">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
@@ -1260,13 +1256,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H29" s="14" t="s">
-        <v>48</v>
+      <c r="H29" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
@@ -1277,19 +1273,19 @@
         <v>6</v>
       </c>
       <c r="F30" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
       <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1311,8 +1307,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
@@ -1323,19 +1319,19 @@
         <v>2</v>
       </c>
       <c r="F32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
       <c r="C33" s="2" t="s">
         <v>26</v>
       </c>
@@ -1345,18 +1341,20 @@
       <c r="E33" s="2">
         <v>1</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
@@ -1366,13 +1364,15 @@
       <c r="E34" s="2">
         <v>1</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1385,13 +1385,15 @@
       <c r="E35" s="2">
         <v>2</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2">
+        <v>2</v>
+      </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1402,8 +1404,8 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="15" t="s">
-        <v>49</v>
+      <c r="H36" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1419,11 +1421,11 @@
       <c r="E37" s="2"/>
       <c r="F37" s="9">
         <f>SUM(F3:F35)</f>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G37" s="10">
         <f>SUM(G3:G35)</f>
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>